<commit_message>
Version 1.0.2 - bug fix in baseline tables
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/ADEPTOBJ1_scripts/definitions/bridge/ADEPT_O1_BRIDGE_19Mayo25.xlsx
+++ b/DEVELOPMENT/ADEPTOBJ1_scripts/definitions/bridge/ADEPT_O1_BRIDGE_19Mayo25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\ADEPT_obj1\DEVELOPMENT\analysis\definitions\bridge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\ADEPT_obj1\DEVELOPMENT\ADEPTOBJ1_scripts\definitions\bridge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0C1D37-499F-41F0-ABD6-A9AAB9DABC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61073D6A-B3C8-4D3C-8D80-D9D337A85730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2506CD93-0285-9E44-BBDD-A2C4E77A0341}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALG!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OBJ1'!$A$1:$K$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'OBJ1'!$A$1:$K$181</definedName>
   </definedNames>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
@@ -2122,14 +2122,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FA1CCF-AC46-4BBB-901E-A0CC50A7045D}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:AB1048576"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2181,7 +2181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>41</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>65</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>71</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>73</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>77</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>79</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>81</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>83</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>85</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>87</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>105</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>107</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>109</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>111</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>115</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>121</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>125</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>127</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>129</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>131</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>133</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>135</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>137</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>139</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>141</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>143</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>151</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>153</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
         <v>167</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>171</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>173</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>177</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>179</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>181</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>183</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>185</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>187</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>189</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>193</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>197</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>199</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>203</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>217</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>225</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>227</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>229</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>231</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>233</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>235</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>239</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>241</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>245</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>247</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>249</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>251</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>267</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>271</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>275</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>277</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>279</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>281</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>283</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>285</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>287</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>289</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>291</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>293</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>85</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>121</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>295</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>297</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>299</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>301</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>303</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>305</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>307</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>309</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>311</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>313</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>315</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>317</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>319</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>321</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>323</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>325</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>327</v>
       </c>
@@ -7820,7 +7820,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>329</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>331</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>333</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>335</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>337</v>
       </c>
@@ -7990,7 +7990,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>339</v>
       </c>
@@ -8025,7 +8025,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>341</v>
       </c>
@@ -8060,7 +8060,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="10" t="s">
         <v>343</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>345</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>347</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>349</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>351</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>353</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="18" t="s">
         <v>361</v>
       </c>
@@ -8389,13 +8389,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K181" xr:uid="{E0FDDF39-709C-C14C-B461-AFB2AA297754}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K181" xr:uid="{E0FDDF39-709C-C14C-B461-AFB2AA297754}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8407,8 +8401,8 @@
   </sheetPr>
   <dimension ref="A1:J171"/>
   <sheetViews>
-    <sheetView topLeftCell="K100" workbookViewId="0">
-      <selection activeCell="C171" sqref="C171"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>